<commit_message>
add home manager script
</commit_message>
<xml_diff>
--- a/Manager/MAPPING.xlsx
+++ b/Manager/MAPPING.xlsx
@@ -176,24 +176,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -207,6 +201,7 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -225,9 +220,9 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>7327</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>7327</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1524000" cy="264560"/>
@@ -268,8 +263,13 @@
         <a:p>
           <a:r>
             <a:rPr lang="fr-FR" sz="1100"/>
-            <a:t>TEST</a:t>
+            <a:t>Géré</a:t>
           </a:r>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
+            <a:t> fenetres</a:t>
+          </a:r>
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -277,9 +277,9 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1524000" cy="761999"/>
@@ -326,12 +326,12 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>14654</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>190499</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="1524000" cy="761999"/>
+    <xdr:ext cx="1524000" cy="771525"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="4" name="ZoneTexte 3"/>
@@ -339,8 +339,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7546731" y="1516673"/>
-          <a:ext cx="1524000" cy="761999"/>
+          <a:off x="7548929" y="1514474"/>
+          <a:ext cx="1524000" cy="771525"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -363,7 +363,7 @@
       </xdr:style>
       <xdr:txBody>
         <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
-          <a:spAutoFit/>
+          <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
@@ -375,12 +375,12 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>14654</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="1524000" cy="609013"/>
+    <xdr:ext cx="1524000" cy="762000"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="5" name="ZoneTexte 4"/>
@@ -388,8 +388,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5832231" y="1516673"/>
-          <a:ext cx="1524000" cy="609013"/>
+          <a:off x="5834429" y="1514475"/>
+          <a:ext cx="1524000" cy="762000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -412,30 +412,10 @@
       </xdr:style>
       <xdr:txBody>
         <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
-          <a:spAutoFit/>
+          <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:r>
-            <a:rPr lang="fr-FR" sz="1100"/>
-            <a:t>Ouvrir:</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="fr-FR" sz="1100"/>
-            <a:t>1</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
-            <a:t> Terminal DIR_Path</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
-            <a:t>1 Github DIR_Path</a:t>
-          </a:r>
           <a:endParaRPr lang="fr-FR" sz="1100"/>
         </a:p>
       </xdr:txBody>
@@ -444,12 +424,12 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>7327</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="1524000" cy="609013"/>
+    <xdr:ext cx="1524000" cy="764198"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="6" name="ZoneTexte 5"/>
@@ -457,8 +437,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4103077" y="1524000"/>
-          <a:ext cx="1524000" cy="609013"/>
+          <a:off x="4105275" y="1521802"/>
+          <a:ext cx="1524000" cy="764198"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -481,30 +461,10 @@
       </xdr:style>
       <xdr:txBody>
         <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
-          <a:spAutoFit/>
+          <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:r>
-            <a:rPr lang="fr-FR" sz="1100"/>
-            <a:t>Ouvrir :</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="fr-FR" sz="1100"/>
-            <a:t>Chrome</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="fr-FR" sz="1100"/>
-            <a:t>VS</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
-            <a:t> Code</a:t>
-          </a:r>
           <a:endParaRPr lang="fr-FR" sz="1100"/>
         </a:p>
       </xdr:txBody>
@@ -513,9 +473,9 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>183173</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>7327</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1524000" cy="264560"/>
@@ -565,9 +525,9 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>175846</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1524000" cy="609013"/>
@@ -617,9 +577,9 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1524000" cy="609013"/>
@@ -674,9 +634,9 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1524000" cy="264560"/>
@@ -731,9 +691,9 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>175846</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>7327</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1524000" cy="436786"/>
@@ -794,9 +754,9 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>14654</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1524000" cy="436786"/>
@@ -851,12 +811,12 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>7327</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>183173</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="1524000" cy="761999"/>
+    <xdr:ext cx="1524000" cy="264560"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="13" name="ZoneTexte 12"/>
@@ -864,8 +824,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9253904" y="3795346"/>
-          <a:ext cx="1524000" cy="761999"/>
+          <a:off x="9256102" y="3793148"/>
+          <a:ext cx="1524000" cy="264560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -892,7 +852,10 @@
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:endParaRPr lang="fr-FR" sz="1100"/>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100"/>
+            <a:t>git SSH</a:t>
+          </a:r>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -900,9 +863,9 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>21981</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>183173</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1524000" cy="264560"/>
@@ -943,7 +906,64 @@
         <a:p>
           <a:r>
             <a:rPr lang="fr-FR" sz="1100"/>
-            <a:t>Git set-url git@...</a:t>
+            <a:t>Git</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
+            <a:t> rm _</a:t>
+          </a:r>
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>21981</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>183173</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1524000" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="ZoneTexte 14"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5841756" y="3793148"/>
+          <a:ext cx="1524000" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100"/>
+            <a:t>Git commit -m "_"</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -952,21 +972,220 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>21981</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>183173</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>7327</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="1524000" cy="761999"/>
+    <xdr:ext cx="1524000" cy="264560"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="15" name="ZoneTexte 14"/>
+        <xdr:cNvPr id="16" name="ZoneTexte 15"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5839558" y="3795346"/>
-          <a:ext cx="1524000" cy="761999"/>
+          <a:off x="4110404" y="3802673"/>
+          <a:ext cx="1524000" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100"/>
+            <a:t>Git add *</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1524000" cy="752475"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="ZoneTexte 16"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10963275" y="4943474"/>
+          <a:ext cx="1524000" cy="752475"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>183173</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>183172</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1524000" cy="769327"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="ZoneTexte 17"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9241448" y="4936147"/>
+          <a:ext cx="1524000" cy="769327"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>7327</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>183172</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1524000" cy="769327"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="19" name="ZoneTexte 18"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7541602" y="4936147"/>
+          <a:ext cx="1524000" cy="769327"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>7327</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>183173</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1524000" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="20" name="ZoneTexte 19"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5827102" y="4936148"/>
+          <a:ext cx="1524000" cy="264560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1002,261 +1221,8 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>7327</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="1524000" cy="264560"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="16" name="ZoneTexte 15"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4110404" y="3802673"/>
-          <a:ext cx="1524000" cy="264560"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
-          <a:spAutoFit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="fr-FR" sz="1100"/>
-            <a:t>Git commit -m</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
-            <a:t> "_"</a:t>
-          </a:r>
-          <a:endParaRPr lang="fr-FR" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="1524000" cy="761999"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="17" name="ZoneTexte 16"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="10961077" y="4945673"/>
-          <a:ext cx="1524000" cy="761999"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
-          <a:spAutoFit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="fr-FR" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>10</xdr:col>
       <xdr:colOff>183173</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>183173</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="1524000" cy="761999"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="18" name="ZoneTexte 17"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9239250" y="4938346"/>
-          <a:ext cx="1524000" cy="761999"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
-          <a:spAutoFit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="fr-FR" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>7327</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>183173</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="1524000" cy="761999"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="19" name="ZoneTexte 18"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7539404" y="4938346"/>
-          <a:ext cx="1524000" cy="761999"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
-          <a:spAutoFit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="fr-FR" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>7327</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>183173</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="1524000" cy="761999"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="20" name="ZoneTexte 19"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5824904" y="4938346"/>
-          <a:ext cx="1524000" cy="761999"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
-          <a:spAutoFit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="fr-FR" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>183173</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1524000" cy="436786"/>
@@ -1312,9 +1278,9 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>7327</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>7327</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1524000" cy="436786"/>
@@ -1364,9 +1330,9 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>7327</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>7327</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1524000" cy="436786"/>
@@ -1422,9 +1388,9 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>183173</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>14654</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1524000" cy="436786"/>
@@ -1773,80 +1739,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD33"/>
+  <dimension ref="A1:AE34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O9" activeCellId="2" sqref="I9:J9 O6:P6 O9:P9"/>
+    <sheetView tabSelected="1" topLeftCell="B2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="58.7109375" customWidth="1"/>
-    <col min="2" max="2" width="2.85546875" customWidth="1"/>
-    <col min="3" max="4" width="11.42578125" customWidth="1"/>
-    <col min="5" max="5" width="2.85546875" style="2" customWidth="1"/>
-    <col min="6" max="7" width="11.42578125" customWidth="1"/>
-    <col min="8" max="8" width="2.85546875" customWidth="1"/>
-    <col min="9" max="10" width="11.42578125" customWidth="1"/>
-    <col min="11" max="11" width="2.85546875" customWidth="1"/>
-    <col min="12" max="13" width="11.42578125" customWidth="1"/>
-    <col min="14" max="14" width="2.85546875" customWidth="1"/>
-    <col min="15" max="16" width="11.42578125" customWidth="1"/>
-    <col min="17" max="17" width="2.85546875" customWidth="1"/>
+    <col min="2" max="3" width="2.85546875" customWidth="1"/>
+    <col min="4" max="5" width="11.42578125" customWidth="1"/>
+    <col min="6" max="6" width="2.85546875" style="2" customWidth="1"/>
+    <col min="7" max="8" width="11.42578125" customWidth="1"/>
+    <col min="9" max="9" width="2.85546875" customWidth="1"/>
+    <col min="10" max="11" width="11.42578125" customWidth="1"/>
+    <col min="12" max="12" width="2.85546875" customWidth="1"/>
+    <col min="13" max="14" width="11.42578125" customWidth="1"/>
+    <col min="15" max="15" width="2.85546875" customWidth="1"/>
+    <col min="16" max="17" width="11.42578125" customWidth="1"/>
+    <col min="18" max="18" width="2.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="3" customFormat="1" ht="89.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="3"/>
-      <c r="S2" s="3"/>
-      <c r="T2" s="3"/>
-      <c r="U2" s="3"/>
-      <c r="V2" s="3"/>
-      <c r="W2" s="3"/>
-      <c r="X2" s="3"/>
-      <c r="Y2" s="3"/>
-      <c r="Z2" s="3"/>
-      <c r="AA2" s="3"/>
-      <c r="AB2" s="3"/>
-      <c r="AC2" s="3"/>
-      <c r="AD2" s="3"/>
-    </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" s="3" customFormat="1" ht="89.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:31" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="23"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
       <c r="E3" s="1"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="23"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
       <c r="H3" s="1"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="6"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
       <c r="K3" s="1"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="6"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
       <c r="N3" s="1"/>
-      <c r="O3" s="24"/>
-      <c r="P3" s="25"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
-      <c r="R3" s="3"/>
+      <c r="R3" s="1"/>
       <c r="S3" s="3"/>
       <c r="T3" s="3"/>
       <c r="U3" s="3"/>
@@ -1859,28 +1794,27 @@
       <c r="AB3" s="3"/>
       <c r="AC3" s="3"/>
       <c r="AD3" s="3"/>
-    </row>
-    <row r="4" spans="1:30" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="8"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="7"/>
-      <c r="P4" s="8"/>
-      <c r="Q4" s="1"/>
-      <c r="R4" s="3"/>
+      <c r="AE3" s="3"/>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="17"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="20"/>
+      <c r="N4" s="17"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="20"/>
+      <c r="Q4" s="17"/>
+      <c r="R4" s="1"/>
       <c r="S4" s="3"/>
       <c r="T4" s="3"/>
       <c r="U4" s="3"/>
@@ -1893,26 +1827,29 @@
       <c r="AB4" s="3"/>
       <c r="AC4" s="3"/>
       <c r="AD4" s="3"/>
-    </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="1"/>
+      <c r="AE4" s="3"/>
+    </row>
+    <row r="5" spans="1:31" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="15"/>
       <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="6"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="6"/>
       <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="6"/>
       <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="6"/>
       <c r="O5" s="1"/>
-      <c r="P5" s="1"/>
-      <c r="Q5" s="1"/>
-      <c r="R5" s="3"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="1"/>
       <c r="S5" s="3"/>
       <c r="T5" s="3"/>
       <c r="U5" s="3"/>
@@ -1925,26 +1862,27 @@
       <c r="AB5" s="3"/>
       <c r="AC5" s="3"/>
       <c r="AD5" s="3"/>
-    </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE5" s="3"/>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="25"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
       <c r="E6" s="1"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="25"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
       <c r="H6" s="1"/>
-      <c r="I6" s="24"/>
-      <c r="J6" s="25"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
       <c r="K6" s="1"/>
-      <c r="L6" s="24"/>
-      <c r="M6" s="25"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
       <c r="N6" s="1"/>
-      <c r="O6" s="24"/>
-      <c r="P6" s="25"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
-      <c r="R6" s="3"/>
+      <c r="R6" s="1"/>
       <c r="S6" s="3"/>
       <c r="T6" s="3"/>
       <c r="U6" s="3"/>
@@ -1957,28 +1895,27 @@
       <c r="AB6" s="3"/>
       <c r="AC6" s="3"/>
       <c r="AD6" s="3"/>
-    </row>
-    <row r="7" spans="1:30" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="9"/>
-      <c r="M7" s="10"/>
-      <c r="N7" s="1"/>
-      <c r="O7" s="9"/>
-      <c r="P7" s="10"/>
-      <c r="Q7" s="1"/>
-      <c r="R7" s="3"/>
+      <c r="AE6" s="3"/>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="18"/>
+      <c r="N7" s="19"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="18"/>
+      <c r="Q7" s="19"/>
+      <c r="R7" s="1"/>
       <c r="S7" s="3"/>
       <c r="T7" s="3"/>
       <c r="U7" s="3"/>
@@ -1991,26 +1928,29 @@
       <c r="AB7" s="3"/>
       <c r="AC7" s="3"/>
       <c r="AD7" s="3"/>
-    </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="1"/>
+      <c r="AE7" s="3"/>
+    </row>
+    <row r="8" spans="1:31" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="16"/>
       <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="8"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="8"/>
       <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="8"/>
       <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="8"/>
       <c r="O8" s="1"/>
-      <c r="P8" s="1"/>
-      <c r="Q8" s="1"/>
-      <c r="R8" s="3"/>
+      <c r="P8" s="7"/>
+      <c r="Q8" s="8"/>
+      <c r="R8" s="1"/>
       <c r="S8" s="3"/>
       <c r="T8" s="3"/>
       <c r="U8" s="3"/>
@@ -2023,26 +1963,27 @@
       <c r="AB8" s="3"/>
       <c r="AC8" s="3"/>
       <c r="AD8" s="3"/>
-    </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE8" s="3"/>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="25"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="12"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
       <c r="H9" s="1"/>
-      <c r="I9" s="24"/>
-      <c r="J9" s="25"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
       <c r="K9" s="1"/>
-      <c r="L9" s="11"/>
-      <c r="M9" s="12"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
       <c r="N9" s="1"/>
-      <c r="O9" s="24"/>
-      <c r="P9" s="25"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
-      <c r="R9" s="3"/>
+      <c r="R9" s="1"/>
       <c r="S9" s="3"/>
       <c r="T9" s="3"/>
       <c r="U9" s="3"/>
@@ -2055,28 +1996,27 @@
       <c r="AB9" s="3"/>
       <c r="AC9" s="3"/>
       <c r="AD9" s="3"/>
-    </row>
-    <row r="10" spans="1:30" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="14"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="13"/>
-      <c r="P10" s="14"/>
-      <c r="Q10" s="1"/>
-      <c r="R10" s="3"/>
+      <c r="AE9" s="3"/>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="19"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="18"/>
+      <c r="N10" s="19"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="18"/>
+      <c r="Q10" s="19"/>
+      <c r="R10" s="1"/>
       <c r="S10" s="3"/>
       <c r="T10" s="3"/>
       <c r="U10" s="3"/>
@@ -2089,26 +2029,29 @@
       <c r="AB10" s="3"/>
       <c r="AC10" s="3"/>
       <c r="AD10" s="3"/>
-    </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="1"/>
+      <c r="AE10" s="3"/>
+    </row>
+    <row r="11" spans="1:31" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="16"/>
       <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="10"/>
       <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="10"/>
       <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="10"/>
       <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="10"/>
       <c r="O11" s="1"/>
-      <c r="P11" s="1"/>
-      <c r="Q11" s="1"/>
-      <c r="R11" s="3"/>
+      <c r="P11" s="9"/>
+      <c r="Q11" s="10"/>
+      <c r="R11" s="1"/>
       <c r="S11" s="3"/>
       <c r="T11" s="3"/>
       <c r="U11" s="3"/>
@@ -2121,26 +2064,27 @@
       <c r="AB11" s="3"/>
       <c r="AC11" s="3"/>
       <c r="AD11" s="3"/>
-    </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE11" s="3"/>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="25"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
       <c r="E12" s="1"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="16"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
       <c r="H12" s="1"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="16"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
       <c r="K12" s="1"/>
-      <c r="L12" s="15"/>
-      <c r="M12" s="16"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
       <c r="N12" s="1"/>
-      <c r="O12" s="15"/>
-      <c r="P12" s="16"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
-      <c r="R12" s="3"/>
+      <c r="R12" s="1"/>
       <c r="S12" s="3"/>
       <c r="T12" s="3"/>
       <c r="U12" s="3"/>
@@ -2153,28 +2097,27 @@
       <c r="AB12" s="3"/>
       <c r="AC12" s="3"/>
       <c r="AD12" s="3"/>
-    </row>
-    <row r="13" spans="1:30" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="17"/>
+      <c r="AE12" s="3"/>
+    </row>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="1"/>
       <c r="D13" s="18"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="17"/>
-      <c r="J13" s="18"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="17"/>
-      <c r="M13" s="18"/>
-      <c r="N13" s="1"/>
-      <c r="O13" s="17"/>
-      <c r="P13" s="18"/>
-      <c r="Q13" s="1"/>
-      <c r="R13" s="3"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="17"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="20"/>
+      <c r="N13" s="17"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="20"/>
+      <c r="Q13" s="17"/>
+      <c r="R13" s="1"/>
       <c r="S13" s="3"/>
       <c r="T13" s="3"/>
       <c r="U13" s="3"/>
@@ -2187,26 +2130,29 @@
       <c r="AB13" s="3"/>
       <c r="AC13" s="3"/>
       <c r="AD13" s="3"/>
-    </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="1"/>
+      <c r="AE13" s="3"/>
+    </row>
+    <row r="14" spans="1:31" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="16"/>
       <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="12"/>
       <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="12"/>
       <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="12"/>
       <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
-      <c r="N14" s="1"/>
+      <c r="M14" s="11"/>
+      <c r="N14" s="12"/>
       <c r="O14" s="1"/>
-      <c r="P14" s="1"/>
-      <c r="Q14" s="1"/>
-      <c r="R14" s="3"/>
+      <c r="P14" s="11"/>
+      <c r="Q14" s="12"/>
+      <c r="R14" s="1"/>
       <c r="S14" s="3"/>
       <c r="T14" s="3"/>
       <c r="U14" s="3"/>
@@ -2219,26 +2165,27 @@
       <c r="AB14" s="3"/>
       <c r="AC14" s="3"/>
       <c r="AD14" s="3"/>
-    </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE14" s="3"/>
+    </row>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="25"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
       <c r="E15" s="1"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="25"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
       <c r="H15" s="1"/>
-      <c r="I15" s="24"/>
-      <c r="J15" s="25"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
       <c r="K15" s="1"/>
-      <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
-      <c r="N15" s="4"/>
-      <c r="O15" s="4"/>
-      <c r="P15" s="4"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
-      <c r="R15" s="3"/>
+      <c r="R15" s="1"/>
       <c r="S15" s="3"/>
       <c r="T15" s="3"/>
       <c r="U15" s="3"/>
@@ -2251,28 +2198,27 @@
       <c r="AB15" s="3"/>
       <c r="AC15" s="3"/>
       <c r="AD15" s="3"/>
-    </row>
-    <row r="16" spans="1:30" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" s="1"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="19"/>
-      <c r="J16" s="20"/>
-      <c r="K16" s="1"/>
+      <c r="AE15" s="3"/>
+    </row>
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="18"/>
+      <c r="K16" s="19"/>
       <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
-      <c r="N16" s="1"/>
-      <c r="O16" s="1"/>
-      <c r="P16" s="1"/>
-      <c r="Q16" s="1"/>
-      <c r="R16" s="3"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="4"/>
+      <c r="O16" s="4"/>
+      <c r="P16" s="4"/>
+      <c r="Q16" s="4"/>
+      <c r="R16" s="1"/>
       <c r="S16" s="3"/>
       <c r="T16" s="3"/>
       <c r="U16" s="3"/>
@@ -2285,26 +2231,29 @@
       <c r="AB16" s="3"/>
       <c r="AC16" s="3"/>
       <c r="AD16" s="3"/>
-    </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
-      <c r="B17" s="1"/>
+      <c r="AE16" s="3"/>
+    </row>
+    <row r="17" spans="1:31" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="16"/>
       <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="14"/>
       <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="14"/>
       <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="14"/>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
-      <c r="R17" s="3"/>
+      <c r="R17" s="1"/>
       <c r="S17" s="3"/>
       <c r="T17" s="3"/>
       <c r="U17" s="3"/>
@@ -2317,26 +2266,27 @@
       <c r="AB17" s="3"/>
       <c r="AC17" s="3"/>
       <c r="AD17" s="3"/>
-    </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE17" s="3"/>
+    </row>
+    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
-      <c r="M18" s="3"/>
-      <c r="N18" s="3"/>
-      <c r="O18" s="3"/>
-      <c r="P18" s="3"/>
-      <c r="Q18" s="3"/>
-      <c r="R18" s="3"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
       <c r="S18" s="3"/>
       <c r="T18" s="3"/>
       <c r="U18" s="3"/>
@@ -2349,8 +2299,9 @@
       <c r="AB18" s="3"/>
       <c r="AC18" s="3"/>
       <c r="AD18" s="3"/>
-    </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE18" s="3"/>
+    </row>
+    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -2381,8 +2332,9 @@
       <c r="AB19" s="3"/>
       <c r="AC19" s="3"/>
       <c r="AD19" s="3"/>
-    </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE19" s="3"/>
+    </row>
+    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -2413,8 +2365,9 @@
       <c r="AB20" s="3"/>
       <c r="AC20" s="3"/>
       <c r="AD20" s="3"/>
-    </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE20" s="3"/>
+    </row>
+    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -2445,8 +2398,9 @@
       <c r="AB21" s="3"/>
       <c r="AC21" s="3"/>
       <c r="AD21" s="3"/>
-    </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE21" s="3"/>
+    </row>
+    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -2477,8 +2431,9 @@
       <c r="AB22" s="3"/>
       <c r="AC22" s="3"/>
       <c r="AD22" s="3"/>
-    </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE22" s="3"/>
+    </row>
+    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -2509,8 +2464,9 @@
       <c r="AB23" s="3"/>
       <c r="AC23" s="3"/>
       <c r="AD23" s="3"/>
-    </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE23" s="3"/>
+    </row>
+    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -2541,8 +2497,9 @@
       <c r="AB24" s="3"/>
       <c r="AC24" s="3"/>
       <c r="AD24" s="3"/>
-    </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE24" s="3"/>
+    </row>
+    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -2573,8 +2530,9 @@
       <c r="AB25" s="3"/>
       <c r="AC25" s="3"/>
       <c r="AD25" s="3"/>
-    </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE25" s="3"/>
+    </row>
+    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -2605,8 +2563,9 @@
       <c r="AB26" s="3"/>
       <c r="AC26" s="3"/>
       <c r="AD26" s="3"/>
-    </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE26" s="3"/>
+    </row>
+    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -2637,8 +2596,9 @@
       <c r="AB27" s="3"/>
       <c r="AC27" s="3"/>
       <c r="AD27" s="3"/>
-    </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE27" s="3"/>
+    </row>
+    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -2669,8 +2629,9 @@
       <c r="AB28" s="3"/>
       <c r="AC28" s="3"/>
       <c r="AD28" s="3"/>
-    </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE28" s="3"/>
+    </row>
+    <row r="29" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -2701,8 +2662,9 @@
       <c r="AB29" s="3"/>
       <c r="AC29" s="3"/>
       <c r="AD29" s="3"/>
-    </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE29" s="3"/>
+    </row>
+    <row r="30" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -2733,8 +2695,9 @@
       <c r="AB30" s="3"/>
       <c r="AC30" s="3"/>
       <c r="AD30" s="3"/>
-    </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE30" s="3"/>
+    </row>
+    <row r="31" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -2765,8 +2728,9 @@
       <c r="AB31" s="3"/>
       <c r="AC31" s="3"/>
       <c r="AD31" s="3"/>
-    </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE31" s="3"/>
+    </row>
+    <row r="32" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -2797,8 +2761,9 @@
       <c r="AB32" s="3"/>
       <c r="AC32" s="3"/>
       <c r="AD32" s="3"/>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="AE32" s="3"/>
+    </row>
+    <row r="33" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -2817,6 +2782,40 @@
       <c r="P33" s="3"/>
       <c r="Q33" s="3"/>
       <c r="R33" s="3"/>
+      <c r="S33" s="3"/>
+      <c r="T33" s="3"/>
+      <c r="U33" s="3"/>
+      <c r="V33" s="3"/>
+      <c r="W33" s="3"/>
+      <c r="X33" s="3"/>
+      <c r="Y33" s="3"/>
+      <c r="Z33" s="3"/>
+      <c r="AA33" s="3"/>
+      <c r="AB33" s="3"/>
+      <c r="AC33" s="3"/>
+      <c r="AD33" s="3"/>
+      <c r="AE33" s="3"/>
+    </row>
+    <row r="34" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A34" s="3"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="3"/>
+      <c r="J34" s="3"/>
+      <c r="K34" s="3"/>
+      <c r="L34" s="3"/>
+      <c r="M34" s="3"/>
+      <c r="N34" s="3"/>
+      <c r="O34" s="3"/>
+      <c r="P34" s="3"/>
+      <c r="Q34" s="3"/>
+      <c r="R34" s="3"/>
+      <c r="S34" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>